<commit_message>
changed direction to web app
</commit_message>
<xml_diff>
--- a/financial_projection.xlsx
+++ b/financial_projection.xlsx
@@ -50,8 +50,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00B6D7A8"/>
-        <bgColor rgb="00B6D7A8"/>
+        <fgColor rgb="0087CEEB"/>
+        <bgColor rgb="0087CEEB"/>
       </patternFill>
     </fill>
     <fill>
@@ -729,7 +729,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45382.04388262732</v>
+        <v>45382.9414271412</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -974,7 +974,7 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45412.04388262732</v>
+        <v>45412.9414271412</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1219,7 +1219,7 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45442.04388262732</v>
+        <v>45442.9414271412</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>

</xml_diff>